<commit_message>
Added extra comments regarding empty bags in efficiency sheet
</commit_message>
<xml_diff>
--- a/efficiency.xlsx
+++ b/efficiency.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
   <si>
     <t>Jacob Alonzo, Samuel Araya, Manan Patel</t>
   </si>
@@ -85,166 +85,175 @@
     <t>Union Best Case: O(n)</t>
   </si>
   <si>
+    <t xml:space="preserve">The Big O Notation for best case and worse case for union do not change since all elements need to be added. </t>
+  </si>
+  <si>
+    <t>(this is the best case assuming no empty bags, if we had empty bags the Big O Notation would be O(1) depending on which bags are empty)</t>
+  </si>
+  <si>
+    <t>intersection Worst Case: O(n^3)</t>
+  </si>
+  <si>
+    <t>We go through every element in bag2, see if the element in bag2 exists in bag1, and if it does, add it to result and delete that element from bag1.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">To do this we use a </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>for loop</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> that uses an if statement with </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>.contains</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> that when true, runs </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>.remove</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>, so Big O Notation is O(n^3)</t>
+    </r>
+  </si>
+  <si>
+    <t>intersection Best Case: O(2)</t>
+  </si>
+  <si>
+    <t>If we go through every element in bag2, and when we check if the element in bag2 exists in bag1 we learn it never does, we never will call .remove so</t>
+  </si>
+  <si>
+    <t>the Big O Notation is O(n^2). This would happen if the two bags were completely different.</t>
+  </si>
+  <si>
+    <t>(this is the best case assuming no empty bags, if we had empty bags the Big O Notation would be either O(1) or O(n) depending on which bags are empty)</t>
+  </si>
+  <si>
+    <t>Difference Worst Case: O(n^3)</t>
+  </si>
+  <si>
+    <t>We go through every element in bag2, see if the element in bag2 exists in bag1, and if it does, delete that element from bag1. bag1 will be the final result.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">To do this we use a </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>for loop</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> that uses an if statement with </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>.contains</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> that when true, runs </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>.remove</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>, so Big O Notation is O(n^3)</t>
+    </r>
+  </si>
+  <si>
+    <t>Difference Best Case: O(n^2)</t>
+  </si>
+  <si>
+    <t>LinkedBag</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Every element in bag1 and bag2 is added into the result bag in separate </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <i/>
+        <color theme="1"/>
+      </rPr>
+      <t>for and while loops</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>, so Big O Notation is O(n)</t>
+    </r>
+  </si>
+  <si>
     <t>The Big O Notation for best case and worse case for union do not change since all elements need to be added. (assuming no empty bags)</t>
-  </si>
-  <si>
-    <t>intersection Worst Case: O(n^3)</t>
-  </si>
-  <si>
-    <t>We go through every element in bag2, see if the element in bag2 exists in bag1, and if it does, add it to result and delete that element from bag1.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">To do this we use a </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>for loop</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> that uses an if statement with </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>.contains</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> that when true, runs </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>.remove</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>, so Big O Notation is O(n^3)</t>
-    </r>
-  </si>
-  <si>
-    <t>intersection Best Case: O(2)</t>
-  </si>
-  <si>
-    <t>If we go through every element in bag2, and when we check if the element in bag2 exists in bag1 we learn it never does, we never will call .remove so</t>
-  </si>
-  <si>
-    <t>the Big O Notation is O(n^2). This would happen if the two bags were completely different.</t>
-  </si>
-  <si>
-    <t>Difference Worst Case: O(n^3)</t>
-  </si>
-  <si>
-    <t>We go through every element in bag2, see if the element in bag2 exists in bag1, and if it does, delete that element from bag1. bag1 will be the final result.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">To do this we use a </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>for loop</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> that uses an if statement with </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>.contains</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> that when true, runs </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>.remove</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>, so Big O Notation is O(n^3)</t>
-    </r>
-  </si>
-  <si>
-    <t>Difference Best Case: O(n^2)</t>
-  </si>
-  <si>
-    <t>LinkedBag</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Every element in bag1 and bag2 is added into the result bag in separate </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
-      </rPr>
-      <t>for and while loops</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>, so Big O Notation is O(n)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -575,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -619,14 +628,17 @@
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="16" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="15" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -635,21 +647,25 @@
     <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="17" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="18" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -1018,94 +1034,96 @@
       <c r="B12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="23"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
     </row>
     <row r="13">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="23"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="J16" s="31"/>
+      <c r="B16" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17">
-      <c r="B17" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20">
       <c r="B20" s="25" t="s">
@@ -1124,70 +1142,70 @@
       <c r="B21" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="27"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
     </row>
     <row r="23">
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="J23" s="31"/>
+      <c r="B23" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24">
-      <c r="B24" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
+      <c r="B24" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25">
-      <c r="B25" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="23"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="J25" s="35"/>
     </row>
     <row r="26">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="23"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
     </row>
     <row r="27">
       <c r="B27" s="25" t="s">
@@ -1203,8 +1221,8 @@
       <c r="J27" s="27"/>
     </row>
     <row r="28">
-      <c r="B28" s="28" t="s">
-        <v>22</v>
+      <c r="B28" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
@@ -1216,148 +1234,150 @@
       <c r="J28" s="27"/>
     </row>
     <row r="29">
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="30"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
-    </row>
-    <row r="30">
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31">
-      <c r="B31" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="30"/>
     </row>
     <row r="32">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="42"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="23"/>
-    </row>
-    <row r="33">
-      <c r="B33" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="25" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="24"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="27"/>
-    </row>
-    <row r="35">
-      <c r="B35" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
-    </row>
-    <row r="36">
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="J36" s="31"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="21" t="s">
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="30"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="23"/>
-    </row>
-    <row r="38">
-      <c r="B38" s="24" t="s">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="30"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="38"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="J40" s="35"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="23"/>
-    </row>
-    <row r="39">
-      <c r="B39" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="23"/>
-    </row>
-    <row r="40">
-      <c r="B40" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="27"/>
-    </row>
-    <row r="41">
-      <c r="B41" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
@@ -1366,11 +1386,11 @@
       <c r="J41" s="27"/>
     </row>
     <row r="42">
-      <c r="B42" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
+      <c r="B42" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
@@ -1379,94 +1399,172 @@
       <c r="J42" s="27"/>
     </row>
     <row r="43">
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="J43" s="31"/>
+      <c r="B43" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44">
-      <c r="B44" s="21" t="s">
+      <c r="B44" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="30"/>
+    </row>
+    <row r="45">
+      <c r="B45" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="23"/>
-    </row>
-    <row r="45">
-      <c r="B45" s="24" t="s">
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="30"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="23"/>
-    </row>
-    <row r="46">
-      <c r="B46" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="23"/>
-    </row>
-    <row r="47">
-      <c r="B47" s="25" t="s">
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="30"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="38"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="J48" s="35"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-    </row>
-    <row r="48">
-      <c r="B48" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27"/>
-    </row>
-    <row r="49">
-      <c r="B49" s="34" t="s">
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="27"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="30"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="37"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="30"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="30"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:I5"/>

</xml_diff>